<commit_message>
Updated. Possible Hardware issue with PCB seems unrelated to code. Everything else works fine.
</commit_message>
<xml_diff>
--- a/Ads1299_defRegs.xlsx
+++ b/Ads1299_defRegs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahmood31\Google Drive\nRF5_SDK_13.1.0\examples\_my_projects\nRF52_ADS1299_ExG_MPU9250\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahmood31\Google Drive\nRF5_SDK_13.1.0\examples\_my_projects\nRF52_ADS1299_2CH_EEG\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -712,7 +712,7 @@
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +777,7 @@
       </c>
       <c r="C2" t="str">
         <f>"0x"&amp;TEXT(DEC2HEX(K2+2*J2+4*I2+8*H2+16*G2+32*F2+64*E2+128*D2,2),"00")</f>
-        <v>0x91</v>
+        <v>0x96</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
@@ -795,13 +795,13 @@
         <v>0</v>
       </c>
       <c r="I2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="4">
         <v>45</v>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>0x01</v>
+        <v>0x03</v>
       </c>
       <c r="D14" s="11">
         <v>0</v>
@@ -1302,7 +1302,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="4">
         <v>1</v>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>0x01</v>
+        <v>0x03</v>
       </c>
       <c r="D15" s="11">
         <v>0</v>
@@ -1344,7 +1344,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="4">
         <v>1</v>

</xml_diff>